<commit_message>
Spelling and Grammar changes.
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohman-Docker/html/mitchellgohman.local/express-routes/portfolio/items/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/mitchellgohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED039BF-542F-5A4C-8DB8-BD546A566045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DAA8B5-CC0E-7D45-AD12-5D5B20221AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Develop and maintain their Web application and Wordpress CMS. The apps I have developed here support online bidding for their quarterly Auctions. This involves adding new lots, changing to the various states of the auction (upcoming, current, post, and past). Interactive lot naviagtor with gallery to support multiple images and zoming needs. As well as lot specific states for costs, price realized, and selling now. Currently in the process of converting their Wordpress Front facing website into React, Redux, and Laravel Front End with backend API. Removing third party plugins to connect to authorize.net for purchasing catalogues and auction related transactions.</t>
-  </si>
-  <si>
-    <t>This application has been through many iterations throughout my life as a web developer. I have used to to teach my Web Development courses, and as a way to play with tools I may not otherwise get to work with. It is a full blown Learning Management System with Admin backend  that supports registering for courses, assignment submissions, grading and grade reports, structured content for syllabus, session outline, and resource sharing.</t>
   </si>
   <si>
     <t>My wife's portfolio Website. She designs, I develop. I may have a bias as well, but she is an amazing designer. Her attention to details, spatial relatonships, color and typography is not common knowledge. We have also worked on several web sites where she created the designs/mocks/assets and I translated her vision into html, css, and javascript.</t>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>This application has been through many iterations throughout my life as a web developer. I have used to teach my Web Development courses, and as a way to play with tools I may not otherwise get to work with. It is a full blown Learning Management System with Admin backend  that supports registering for courses, assignment submissions, grading and grade reports, structured content for syllabus, session outline, and resource sharing.</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1221,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
@@ -1239,10 +1239,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1330,7 +1330,7 @@
         <v>86</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1359,10 +1359,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1388,10 +1388,10 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>21</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1420,7 +1420,7 @@
         <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>24</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1449,7 +1449,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -1466,7 +1466,7 @@
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1481,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>32</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -1513,7 +1513,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>28</v>
@@ -1528,12 +1528,12 @@
         <v>13</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1548,7 +1548,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>39</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="11" spans="1:13" ht="18" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1580,7 +1580,7 @@
         <v>42</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>28</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -1612,7 +1612,7 @@
         <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>28</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="13" spans="1:13" ht="18" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1647,10 +1647,10 @@
         <v>51</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>52</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="14" spans="1:13" ht="18" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1679,10 +1679,10 @@
         <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>55</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1711,7 +1711,7 @@
         <v>64</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>28</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
@@ -1743,10 +1743,10 @@
         <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>58</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -1778,10 +1778,10 @@
         <v>61</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>62</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
@@ -1810,10 +1810,10 @@
         <v>67</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>68</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="19" spans="1:12" ht="18" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
@@ -1842,7 +1842,7 @@
         <v>70</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>71</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
@@ -1874,7 +1874,7 @@
         <v>74</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>75</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -1903,7 +1903,7 @@
         <v>78</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Updating Portfolio Items spreadsheet csv conversion to json
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/mitchellgohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DAA8B5-CC0E-7D45-AD12-5D5B20221AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9B394530-4268-AB4E-865C-79A21B159529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
   <si>
     <t>showHide</t>
   </si>
@@ -79,9 +79,6 @@
     <t>ctm.jpg</t>
   </si>
   <si>
-    <t>ctm.com</t>
-  </si>
-  <si>
     <t>Enspyred LMS</t>
   </si>
   <si>
@@ -317,10 +314,6 @@
   </si>
   <si>
     <t>Custom web applicaton using out of the box php, mysql, javascript, html and css.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;My wife, (&lt;a href='https://christinagohman.com' target='xtina'&gt;Christina Gohman&lt;/a&gt;) desaigned and I developed this Wordpress Custom theme for our Wedding. &lt;/&gt;
-&lt;p&gt;It was used to keep all of our guests informed, and boy did that make all the difference in the world. Still one of my favorite designs, is that cause it was my wedding? Nah.&lt;/p&gt; </t>
   </si>
   <si>
     <t>Converted web application to React/Redux/Context. Also employs front and back servers for security, Authorize.net shopping cart for Catlogue order form, Bidding Application,. Laravel, Laravel Corcel Wordpress, Styled-Components, Less, Custom Theme, HTML, CSS, MYSQL, Mongo, Redis Caching, Responsive and Mobile First, Custom Wordpress CMS Plugin</t>
@@ -366,12 +359,19 @@
   <si>
     <t>This application has been through many iterations throughout my life as a web developer. I have used to teach my Web Development courses, and as a way to play with tools I may not otherwise get to work with. It is a full blown Learning Management System with Admin backend  that supports registering for courses, assignment submissions, grading and grade reports, structured content for syllabus, session outline, and resource sharing.</t>
   </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;My wife, (&lt;a href='https://christinagohman.com' target='xtina'&gt;Christina Gohman&lt;/a&gt;) designed and I developed this Wordpress Custom theme for our Wedding. &lt;/&gt;
+&lt;p&gt;It was used to keep all of our guests informed, and boy did that make all the difference in the world. Still one of my favorite designs, is that cause it was my wedding? Nah.&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>travelctm.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1219,16 +1219,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="45" style="1" customWidth="1"/>
-    <col min="6" max="7" width="88" style="2" customWidth="1"/>
+    <col min="6" max="6" width="112.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="88" style="2" customWidth="1"/>
     <col min="8" max="8" width="45.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="58.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="69.1640625" style="1" customWidth="1"/>
@@ -1237,12 +1238,12 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1257,13 +1258,13 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>5</v>
@@ -1278,9 +1279,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18" customHeight="1">
+    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1295,10 +1296,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -1310,9 +1311,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1">
+    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1327,10 +1328,10 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -1342,9 +1343,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1">
+    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1353,27 +1354,30 @@
         <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="18" customHeight="1">
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1385,27 +1389,27 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1">
+    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
@@ -1417,24 +1421,24 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="18" customHeight="1">
+    </row>
+    <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1446,27 +1450,27 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1">
+    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1478,62 +1482,62 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18" customHeight="1">
+    <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1545,27 +1549,27 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18" customHeight="1">
+    <row r="11" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1577,62 +1581,62 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" customHeight="1">
+    <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1">
+    </row>
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -1644,27 +1648,27 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18" customHeight="1">
+    <row r="14" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
@@ -1676,27 +1680,27 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1">
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
@@ -1708,62 +1712,62 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18" customHeight="1">
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1">
+    </row>
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
@@ -1775,144 +1779,144 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" customHeight="1">
+    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1">
+    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1">
+    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="18" customHeight="1">
+    </row>
+    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>13</v>
@@ -1920,5 +1924,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Data to add 2 new portfolio items
</commit_message>
<xml_diff>
--- a/express-routes/portfolio/items/items.xlsx
+++ b/express-routes/portfolio/items/items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/Gohmans/mitchellgohman.local/express-routes/portfolio/items/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meatch/MeatchPod/WEBWORKS/GOHMANS/mitchellgohman.local/express-routes/portfolio/items/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9B394530-4268-AB4E-865C-79A21B159529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C6C8F8-920C-6248-BF08-910C6234BB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="27220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="117">
   <si>
     <t>showHide</t>
   </si>
@@ -365,6 +365,33 @@
   </si>
   <si>
     <t>travelctm.com</t>
+  </si>
+  <si>
+    <t>assessment-rank-items.jpg8</t>
+  </si>
+  <si>
+    <t>assessment-results.jpg8</t>
+  </si>
+  <si>
+    <t>fantastic-four.enspyred.com/rank-items-example</t>
+  </si>
+  <si>
+    <t>fantastic-four.enspyred.com/results-composite-example</t>
+  </si>
+  <si>
+    <t>React/Redux/Context, NodeJS/Express</t>
+  </si>
+  <si>
+    <t>Assessment Project: Rank Items</t>
+  </si>
+  <si>
+    <t>Assessment Project:Assessment Results</t>
+  </si>
+  <si>
+    <t>Assisting in developing an Assessment Apoplication requiring a custom Ranking System.</t>
+  </si>
+  <si>
+    <t>Assisting in developing an Assessment Apoplication requiring a custom SVG results to showcase user's evaluation</t>
   </si>
 </sst>
 </file>
@@ -921,7 +948,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1209,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1217,11 +1244,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1229,7 +1256,7 @@
     <col min="1" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="45" style="1" customWidth="1"/>
     <col min="6" max="6" width="112.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="88" style="2" customWidth="1"/>
+    <col min="7" max="7" width="104.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="45.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="58.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="69.1640625" style="1" customWidth="1"/>
@@ -1293,19 +1320,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -1325,19 +1352,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>13</v>
@@ -1357,19 +1384,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>107</v>
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>13</v>
@@ -1389,19 +1416,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>13</v>
@@ -1421,19 +1448,22 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1450,19 +1480,19 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>13</v>
@@ -1482,22 +1512,19 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1508,31 +1535,28 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1546,24 +1570,24 @@
         <v>9</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1575,28 +1599,31 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1607,31 +1634,28 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1648,19 +1672,19 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>13</v>
@@ -1674,28 +1698,31 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1709,24 +1736,24 @@
         <v>9</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1738,34 +1765,31 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>100</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>103</v>
       </c>
@@ -1776,28 +1800,28 @@
         <v>9</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1811,7 +1835,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>95</v>
@@ -1820,16 +1844,19 @@
         <v>100</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -1837,31 +1864,31 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>103</v>
       </c>
@@ -1875,22 +1902,25 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
@@ -1904,21 +1934,82 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>